<commit_message>
implemented rule-based reactive and opponent utility args
</commit_message>
<xml_diff>
--- a/zsceval/scripts/overcooked/eval/results/random3_m/bias/event_count_hsp_plate_placement_shared.xlsx
+++ b/zsceval/scripts/overcooked/eval/results/random3_m/bias/event_count_hsp_plate_placement_shared.xlsx
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6.675</v>
+        <v>7.1</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -865,142 +865,142 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="K2" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>70</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>313.475</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>15.525</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>6.875</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="n">
         <v>0.05</v>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="K2" t="n">
-        <v>7.55</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="AL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>6.825</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>7.325</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="n">
         <v>0.05</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>74.825</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>309.625</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>11</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>6.625</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>6.55</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>7.55</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>0.025</v>
       </c>
       <c r="AY2" t="n">
         <v>0.175</v>
       </c>
       <c r="AZ2" t="n">
-        <v>8.35</v>
+        <v>8.1</v>
       </c>
       <c r="BA2" t="n">
         <v>0</v>
@@ -1048,13 +1048,13 @@
         <v>0</v>
       </c>
       <c r="BP2" t="n">
-        <v>70.075</v>
+        <v>65.34999999999999</v>
       </c>
       <c r="BQ2" t="n">
-        <v>312.9</v>
+        <v>318.3</v>
       </c>
       <c r="BR2" t="n">
-        <v>13.175</v>
+        <v>13.35</v>
       </c>
       <c r="BS2" t="n">
         <v>0</v>
@@ -1066,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="BV2" t="n">
-        <v>7.4</v>
+        <v>7.175</v>
       </c>
       <c r="BW2" t="n">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="CD2" t="n">
-        <v>7.375</v>
+        <v>7.15</v>
       </c>
       <c r="CE2" t="n">
         <v>0</v>
@@ -1107,28 +1107,28 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>91.27500000000001</v>
+        <v>7.8</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.075</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="J3" t="n">
-        <v>91.425</v>
+        <v>0.075</v>
       </c>
       <c r="K3" t="n">
-        <v>0.125</v>
+        <v>9.25</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -1137,16 +1137,16 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>1.375</v>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>1.375</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>1.375</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
@@ -1155,37 +1155,37 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>0.075</v>
       </c>
       <c r="U3" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="W3" t="n">
-        <v>0</v>
+        <v>0.575</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="Y3" t="n">
         <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>0</v>
+        <v>0.525</v>
       </c>
       <c r="AA3" t="n">
-        <v>9.699999999999999</v>
+        <v>59.925</v>
       </c>
       <c r="AB3" t="n">
-        <v>207.25</v>
+        <v>312.775</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.35</v>
+        <v>10.9</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.225</v>
+        <v>0.375</v>
       </c>
       <c r="AE3" t="n">
         <v>0</v>
@@ -1194,10 +1194,10 @@
         <v>0</v>
       </c>
       <c r="AG3" t="n">
-        <v>87.3</v>
+        <v>7.725</v>
       </c>
       <c r="AH3" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="AI3" t="n">
         <v>0</v>
@@ -1206,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="AK3" t="n">
-        <v>87.45</v>
+        <v>0</v>
       </c>
       <c r="AL3" t="n">
         <v>0</v>
@@ -1218,10 +1218,10 @@
         <v>0</v>
       </c>
       <c r="AO3" t="n">
-        <v>-0.15</v>
+        <v>7.725</v>
       </c>
       <c r="AP3" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="AQ3" t="n">
         <v>0</v>
@@ -1230,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="AS3" t="n">
-        <v>93.84999999999999</v>
+        <v>6.35</v>
       </c>
       <c r="AT3" t="n">
         <v>0</v>
@@ -1239,19 +1239,19 @@
         <v>0</v>
       </c>
       <c r="AV3" t="n">
-        <v>0</v>
+        <v>0.175</v>
       </c>
       <c r="AW3" t="n">
         <v>0</v>
       </c>
       <c r="AX3" t="n">
-        <v>0</v>
+        <v>1.625</v>
       </c>
       <c r="AY3" t="n">
-        <v>87.2</v>
+        <v>0.175</v>
       </c>
       <c r="AZ3" t="n">
-        <v>7</v>
+        <v>8.025</v>
       </c>
       <c r="BA3" t="n">
         <v>0</v>
@@ -1260,52 +1260,52 @@
         <v>0</v>
       </c>
       <c r="BC3" t="n">
-        <v>0</v>
+        <v>1.025</v>
       </c>
       <c r="BD3" t="n">
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="BE3" t="n">
-        <v>0</v>
+        <v>1.725</v>
       </c>
       <c r="BF3" t="n">
-        <v>0</v>
+        <v>1.725</v>
       </c>
       <c r="BG3" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="BH3" t="n">
         <v>0</v>
       </c>
       <c r="BI3" t="n">
-        <v>0</v>
+        <v>0.175</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0</v>
+        <v>1.575</v>
       </c>
       <c r="BK3" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="BL3" t="n">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="BM3" t="n">
-        <v>0</v>
+        <v>0.175</v>
       </c>
       <c r="BN3" t="n">
         <v>0</v>
       </c>
       <c r="BO3" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="BP3" t="n">
-        <v>37.425</v>
+        <v>60.575</v>
       </c>
       <c r="BQ3" t="n">
-        <v>174.525</v>
+        <v>314.275</v>
       </c>
       <c r="BR3" t="n">
-        <v>0.475</v>
+        <v>13.05</v>
       </c>
       <c r="BS3" t="n">
         <v>0</v>
@@ -1317,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="BV3" t="n">
-        <v>90.55</v>
+        <v>6.225</v>
       </c>
       <c r="BW3" t="n">
         <v>0</v>
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="BZ3" t="n">
-        <v>83.90000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="CA3" t="n">
         <v>0</v>
@@ -1341,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="CD3" t="n">
-        <v>6.65</v>
+        <v>6.175</v>
       </c>
       <c r="CE3" t="n">
         <v>0</v>
@@ -1358,7 +1358,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>10.375</v>
+        <v>7.9</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1367,7 +1367,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -1376,10 +1376,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>2.65</v>
+        <v>0.05</v>
       </c>
       <c r="K4" t="n">
-        <v>8.675000000000001</v>
+        <v>8.85</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -1391,13 +1391,13 @@
         <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
@@ -1406,13 +1406,13 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
@@ -1427,13 +1427,13 @@
         <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>76.5</v>
+        <v>77.47499999999999</v>
       </c>
       <c r="AB4" t="n">
-        <v>299.675</v>
+        <v>302.6</v>
       </c>
       <c r="AC4" t="n">
-        <v>8.225</v>
+        <v>5.7</v>
       </c>
       <c r="AD4" t="n">
         <v>0.025</v>
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="AG4" t="n">
-        <v>8.225</v>
+        <v>7.85</v>
       </c>
       <c r="AH4" t="n">
         <v>0</v>
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AL4" t="n">
         <v>0</v>
@@ -1469,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="AO4" t="n">
-        <v>7.725</v>
+        <v>7.85</v>
       </c>
       <c r="AP4" t="n">
         <v>0</v>
@@ -1478,10 +1478,10 @@
         <v>0</v>
       </c>
       <c r="AR4" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="AS4" t="n">
-        <v>9.525</v>
+        <v>6.175</v>
       </c>
       <c r="AT4" t="n">
         <v>0</v>
@@ -1490,98 +1490,98 @@
         <v>0</v>
       </c>
       <c r="AV4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>7</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>75.65000000000001</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>308.5</v>
+      </c>
+      <c r="BR4" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU4" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>6.075</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BZ4" t="n">
         <v>0.075</v>
       </c>
-      <c r="AW4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY4" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="AZ4" t="n">
-        <v>7.3</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD4" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="BF4" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI4" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="BJ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BK4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP4" t="n">
-        <v>77.02500000000001</v>
-      </c>
-      <c r="BQ4" t="n">
-        <v>300.6</v>
-      </c>
-      <c r="BR4" t="n">
-        <v>6.775</v>
-      </c>
-      <c r="BS4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BT4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BV4" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="BW4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BY4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BZ4" t="n">
-        <v>1.075</v>
-      </c>
       <c r="CA4" t="n">
         <v>0</v>
       </c>
@@ -1589,10 +1589,10 @@
         <v>0</v>
       </c>
       <c r="CC4" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="CD4" t="n">
-        <v>6.325</v>
+        <v>6</v>
       </c>
       <c r="CE4" t="n">
         <v>0</v>
@@ -1603,52 +1603,52 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1</v>
+        <v>0.625</v>
       </c>
       <c r="C5" t="n">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1.2</v>
+        <v>0.025</v>
       </c>
       <c r="E5" t="n">
-        <v>0.35</v>
+        <v>0.025</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1</v>
+        <v>0.625</v>
       </c>
       <c r="G5" t="n">
-        <v>1.25</v>
+        <v>9.074999999999999</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>7.075</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>7.575</v>
+        <v>5.4</v>
       </c>
       <c r="L5" t="n">
-        <v>0.225</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>7.575</v>
+        <v>5.325</v>
       </c>
       <c r="N5" t="n">
-        <v>7.075</v>
+        <v>5.275</v>
       </c>
       <c r="O5" t="n">
-        <v>8.125</v>
+        <v>8.925000000000001</v>
       </c>
       <c r="P5" t="n">
-        <v>8.125</v>
+        <v>8.925000000000001</v>
       </c>
       <c r="Q5" t="n">
-        <v>8.125</v>
+        <v>8.925000000000001</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
@@ -1657,196 +1657,196 @@
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>1.25</v>
+        <v>8.925000000000001</v>
       </c>
       <c r="U5" t="n">
-        <v>6.875</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>7.95</v>
+        <v>6.325</v>
       </c>
       <c r="W5" t="n">
-        <v>6.875</v>
+        <v>5.2</v>
       </c>
       <c r="X5" t="n">
-        <v>0.1</v>
+        <v>2.45</v>
       </c>
       <c r="Y5" t="n">
         <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>6.8</v>
+        <v>2.75</v>
       </c>
       <c r="AA5" t="n">
-        <v>49.3</v>
+        <v>47.05</v>
       </c>
       <c r="AB5" t="n">
-        <v>299.8</v>
+        <v>310.375</v>
       </c>
       <c r="AC5" t="n">
-        <v>1.775</v>
+        <v>1.525</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>0</v>
+        <v>0.075</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>9.574999999999999</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>6.125</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>6</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>5.925</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>5.325</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>42.475</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>312.45</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT5" t="n">
         <v>0.15</v>
       </c>
-      <c r="AH5" t="n">
-        <v>0.175</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AP5" t="n">
+      <c r="BU5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="BW5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BZ5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="CA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB5" t="n">
         <v>0.125</v>
       </c>
-      <c r="AQ5" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>7.05</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>1.375</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>1.825</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>7.925</v>
-      </c>
-      <c r="BA5" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="BB5" t="n">
-        <v>7.9</v>
-      </c>
-      <c r="BC5" t="n">
-        <v>7.75</v>
-      </c>
-      <c r="BD5" t="n">
-        <v>8.15</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>8.15</v>
-      </c>
-      <c r="BF5" t="n">
-        <v>8.15</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI5" t="n">
-        <v>6.825</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>1.325</v>
-      </c>
-      <c r="BK5" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="BL5" t="n">
-        <v>7.45</v>
-      </c>
-      <c r="BM5" t="n">
-        <v>0.175</v>
-      </c>
-      <c r="BN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO5" t="n">
-        <v>7.45</v>
-      </c>
-      <c r="BP5" t="n">
-        <v>45.425</v>
-      </c>
-      <c r="BQ5" t="n">
-        <v>298.25</v>
-      </c>
-      <c r="BR5" t="n">
-        <v>1.025</v>
-      </c>
-      <c r="BS5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BU5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BV5" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="BW5" t="n">
-        <v>0.225</v>
-      </c>
-      <c r="BX5" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="BY5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BZ5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="CA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CB5" t="n">
-        <v>-0.025</v>
-      </c>
       <c r="CC5" t="n">
         <v>0</v>
       </c>
       <c r="CD5" t="n">
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="CE5" t="n">
-        <v>0.225</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1860,7 +1860,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>6.75</v>
+        <v>7.875</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1875,13 +1875,13 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="K6" t="n">
-        <v>7.525</v>
+        <v>8.824999999999999</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -1929,16 +1929,16 @@
         <v>0</v>
       </c>
       <c r="AA6" t="n">
-        <v>77.075</v>
+        <v>75.375</v>
       </c>
       <c r="AB6" t="n">
-        <v>306.3</v>
+        <v>305.575</v>
       </c>
       <c r="AC6" t="n">
-        <v>6.425</v>
+        <v>6.325</v>
       </c>
       <c r="AD6" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="AE6" t="n">
         <v>0</v>
@@ -1947,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="AG6" t="n">
-        <v>6.6</v>
+        <v>7.825</v>
       </c>
       <c r="AH6" t="n">
         <v>0</v>
@@ -1959,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="AL6" t="n">
         <v>0</v>
@@ -1971,7 +1971,7 @@
         <v>0</v>
       </c>
       <c r="AO6" t="n">
-        <v>6.55</v>
+        <v>7.825</v>
       </c>
       <c r="AP6" t="n">
         <v>0</v>
@@ -1983,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="AS6" t="n">
-        <v>7.975</v>
+        <v>6.375</v>
       </c>
       <c r="AT6" t="n">
         <v>0</v>
@@ -1998,13 +1998,13 @@
         <v>0</v>
       </c>
       <c r="AX6" t="n">
-        <v>0.05</v>
+        <v>0.025</v>
       </c>
       <c r="AY6" t="n">
-        <v>0.475</v>
+        <v>0.1</v>
       </c>
       <c r="AZ6" t="n">
-        <v>8.5</v>
+        <v>7.25</v>
       </c>
       <c r="BA6" t="n">
         <v>0</v>
@@ -2016,13 +2016,13 @@
         <v>0</v>
       </c>
       <c r="BD6" t="n">
-        <v>0.05</v>
+        <v>0.025</v>
       </c>
       <c r="BE6" t="n">
-        <v>0.05</v>
+        <v>0.025</v>
       </c>
       <c r="BF6" t="n">
-        <v>0.05</v>
+        <v>0.025</v>
       </c>
       <c r="BG6" t="n">
         <v>0</v>
@@ -2034,7 +2034,7 @@
         <v>0</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.05</v>
+        <v>0.025</v>
       </c>
       <c r="BK6" t="n">
         <v>0</v>
@@ -2052,13 +2052,13 @@
         <v>0</v>
       </c>
       <c r="BP6" t="n">
-        <v>74.97499999999999</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="BQ6" t="n">
-        <v>305.1</v>
+        <v>312.075</v>
       </c>
       <c r="BR6" t="n">
-        <v>7.525</v>
+        <v>8.324999999999999</v>
       </c>
       <c r="BS6" t="n">
         <v>0</v>
@@ -2070,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="BV6" t="n">
-        <v>7.625</v>
+        <v>6.375</v>
       </c>
       <c r="BW6" t="n">
         <v>0</v>
@@ -2082,7 +2082,7 @@
         <v>0</v>
       </c>
       <c r="BZ6" t="n">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="CA6" t="n">
         <v>0</v>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="CD6" t="n">
-        <v>7.5</v>
+        <v>6.275</v>
       </c>
       <c r="CE6" t="n">
         <v>0</v>
@@ -2108,10 +2108,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>9.625</v>
+        <v>7.8</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -2126,13 +2126,13 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0.025</v>
+        <v>0.1</v>
       </c>
       <c r="J7" t="n">
-        <v>1.9</v>
+        <v>0.175</v>
       </c>
       <c r="K7" t="n">
-        <v>8.725</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -2144,13 +2144,13 @@
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="P7" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="V7" t="n">
         <v>0</v>
@@ -2180,13 +2180,13 @@
         <v>0</v>
       </c>
       <c r="AA7" t="n">
-        <v>72.375</v>
+        <v>68.97499999999999</v>
       </c>
       <c r="AB7" t="n">
-        <v>304.125</v>
+        <v>312.425</v>
       </c>
       <c r="AC7" t="n">
-        <v>6.775</v>
+        <v>8.125</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
@@ -2195,10 +2195,10 @@
         <v>0</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="AG7" t="n">
-        <v>7.9</v>
+        <v>7.675</v>
       </c>
       <c r="AH7" t="n">
         <v>0</v>
@@ -2210,142 +2210,142 @@
         <v>0</v>
       </c>
       <c r="AK7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>7.625</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>6.575</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>7.325</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>70.875</v>
+      </c>
+      <c r="BQ7" t="n">
+        <v>313.35</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>7.475</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BU7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BV7" t="n">
+        <v>6.525</v>
+      </c>
+      <c r="BW7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BZ7" t="n">
         <v>0.175</v>
       </c>
-      <c r="AL7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN7" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>7.725</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="AR7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS7" t="n">
-        <v>8.175000000000001</v>
-      </c>
-      <c r="AT7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="AW7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX7" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="AY7" t="n">
-        <v>2.075</v>
-      </c>
-      <c r="AZ7" t="n">
-        <v>7.075</v>
-      </c>
-      <c r="BA7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD7" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="BE7" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="BF7" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="BG7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BI7" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="BJ7" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="BK7" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="BL7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP7" t="n">
-        <v>72.90000000000001</v>
-      </c>
-      <c r="BQ7" t="n">
-        <v>307.5</v>
-      </c>
-      <c r="BR7" t="n">
-        <v>8.375</v>
-      </c>
-      <c r="BS7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BT7" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="BU7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BV7" t="n">
-        <v>6.975</v>
-      </c>
-      <c r="BW7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BY7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BZ7" t="n">
-        <v>0.875</v>
-      </c>
       <c r="CA7" t="n">
         <v>0</v>
       </c>
       <c r="CB7" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="CC7" t="n">
         <v>0</v>
       </c>
       <c r="CD7" t="n">
-        <v>6.1</v>
+        <v>6.35</v>
       </c>
       <c r="CE7" t="n">
         <v>0</v>
@@ -2362,7 +2362,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>8.1</v>
+        <v>7.825</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -2371,19 +2371,19 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="K8" t="n">
-        <v>8.875</v>
+        <v>8.775</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -2395,13 +2395,13 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
@@ -2413,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="V8" t="n">
         <v>0</v>
@@ -2431,13 +2431,13 @@
         <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>72.27500000000001</v>
+        <v>74.47499999999999</v>
       </c>
       <c r="AB8" t="n">
-        <v>309.975</v>
+        <v>306.65</v>
       </c>
       <c r="AC8" t="n">
-        <v>5.725</v>
+        <v>5.75</v>
       </c>
       <c r="AD8" t="n">
         <v>0.025</v>
@@ -2449,7 +2449,7 @@
         <v>0</v>
       </c>
       <c r="AG8" t="n">
-        <v>7.925</v>
+        <v>7.775</v>
       </c>
       <c r="AH8" t="n">
         <v>0</v>
@@ -2461,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="AL8" t="n">
         <v>0</v>
@@ -2473,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="AO8" t="n">
-        <v>7.9</v>
+        <v>7.775</v>
       </c>
       <c r="AP8" t="n">
         <v>0</v>
@@ -2482,10 +2482,10 @@
         <v>0</v>
       </c>
       <c r="AR8" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="AS8" t="n">
-        <v>6.3</v>
+        <v>5.975</v>
       </c>
       <c r="AT8" t="n">
         <v>0</v>
@@ -2503,10 +2503,10 @@
         <v>0.075</v>
       </c>
       <c r="AY8" t="n">
-        <v>0.2</v>
+        <v>0.025</v>
       </c>
       <c r="AZ8" t="n">
-        <v>7.05</v>
+        <v>6.9</v>
       </c>
       <c r="BA8" t="n">
         <v>0</v>
@@ -2518,13 +2518,13 @@
         <v>0</v>
       </c>
       <c r="BD8" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="BE8" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="BF8" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="BG8" t="n">
         <v>0</v>
@@ -2536,7 +2536,7 @@
         <v>0</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="BK8" t="n">
         <v>0</v>
@@ -2554,13 +2554,13 @@
         <v>0</v>
       </c>
       <c r="BP8" t="n">
-        <v>74.2</v>
+        <v>77.47499999999999</v>
       </c>
       <c r="BQ8" t="n">
-        <v>311.925</v>
+        <v>308.825</v>
       </c>
       <c r="BR8" t="n">
-        <v>7.475</v>
+        <v>7.825</v>
       </c>
       <c r="BS8" t="n">
         <v>0</v>
@@ -2569,10 +2569,10 @@
         <v>0</v>
       </c>
       <c r="BU8" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="BV8" t="n">
-        <v>6.175</v>
+        <v>5.95</v>
       </c>
       <c r="BW8" t="n">
         <v>0</v>
@@ -2584,7 +2584,7 @@
         <v>0</v>
       </c>
       <c r="BZ8" t="n">
-        <v>0.075</v>
+        <v>0</v>
       </c>
       <c r="CA8" t="n">
         <v>0</v>
@@ -2593,10 +2593,10 @@
         <v>0</v>
       </c>
       <c r="CC8" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="CD8" t="n">
-        <v>6.1</v>
+        <v>5.95</v>
       </c>
       <c r="CE8" t="n">
         <v>0</v>
@@ -2610,10 +2610,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="D9" t="n">
-        <v>105.275</v>
+        <v>6.775</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -2622,19 +2622,19 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>1.875</v>
       </c>
       <c r="J9" t="n">
-        <v>102.575</v>
+        <v>0.1</v>
       </c>
       <c r="K9" t="n">
-        <v>3.025</v>
+        <v>8.625</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
@@ -2643,16 +2643,16 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>2.15</v>
       </c>
       <c r="P9" t="n">
-        <v>0</v>
+        <v>2.15</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>2.15</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
@@ -2661,37 +2661,37 @@
         <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="V9" t="n">
-        <v>0</v>
+        <v>1.775</v>
       </c>
       <c r="W9" t="n">
-        <v>0</v>
+        <v>1.175</v>
       </c>
       <c r="X9" t="n">
-        <v>0</v>
+        <v>0.275</v>
       </c>
       <c r="Y9" t="n">
         <v>0</v>
       </c>
       <c r="Z9" t="n">
-        <v>0</v>
+        <v>1.025</v>
       </c>
       <c r="AA9" t="n">
-        <v>31.225</v>
+        <v>74.7</v>
       </c>
       <c r="AB9" t="n">
-        <v>157.375</v>
+        <v>297.6</v>
       </c>
       <c r="AC9" t="n">
-        <v>4.95</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.525</v>
+        <v>0.025</v>
       </c>
       <c r="AE9" t="n">
         <v>0</v>
@@ -2700,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="AG9" t="n">
-        <v>80.05</v>
+        <v>6.75</v>
       </c>
       <c r="AH9" t="n">
         <v>0</v>
@@ -2712,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="AK9" t="n">
-        <v>77.34999999999999</v>
+        <v>0.075</v>
       </c>
       <c r="AL9" t="n">
         <v>0</v>
@@ -2724,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="AO9" t="n">
-        <v>2.7</v>
+        <v>6.675</v>
       </c>
       <c r="AP9" t="n">
         <v>0</v>
@@ -2736,28 +2736,28 @@
         <v>0</v>
       </c>
       <c r="AS9" t="n">
-        <v>86.45</v>
+        <v>7.475</v>
       </c>
       <c r="AT9" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="AU9" t="n">
         <v>0</v>
       </c>
       <c r="AV9" t="n">
-        <v>0.025</v>
+        <v>0.425</v>
       </c>
       <c r="AW9" t="n">
         <v>0</v>
       </c>
       <c r="AX9" t="n">
-        <v>0</v>
+        <v>1.675</v>
       </c>
       <c r="AY9" t="n">
-        <v>83.7</v>
+        <v>0.075</v>
       </c>
       <c r="AZ9" t="n">
-        <v>3.25</v>
+        <v>9.375</v>
       </c>
       <c r="BA9" t="n">
         <v>0</v>
@@ -2766,16 +2766,16 @@
         <v>0</v>
       </c>
       <c r="BC9" t="n">
-        <v>0</v>
+        <v>1.425</v>
       </c>
       <c r="BD9" t="n">
-        <v>0</v>
+        <v>1.825</v>
       </c>
       <c r="BE9" t="n">
-        <v>0</v>
+        <v>1.825</v>
       </c>
       <c r="BF9" t="n">
-        <v>0</v>
+        <v>1.825</v>
       </c>
       <c r="BG9" t="n">
         <v>0</v>
@@ -2784,34 +2784,34 @@
         <v>0</v>
       </c>
       <c r="BI9" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0</v>
+        <v>1.425</v>
       </c>
       <c r="BK9" t="n">
-        <v>0</v>
+        <v>1.65</v>
       </c>
       <c r="BL9" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="BM9" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="BN9" t="n">
         <v>0</v>
       </c>
       <c r="BO9" t="n">
-        <v>0</v>
+        <v>1.275</v>
       </c>
       <c r="BP9" t="n">
-        <v>80.5</v>
+        <v>71.97499999999999</v>
       </c>
       <c r="BQ9" t="n">
-        <v>146.075</v>
+        <v>300.1</v>
       </c>
       <c r="BR9" t="n">
-        <v>1.2</v>
+        <v>8.975</v>
       </c>
       <c r="BS9" t="n">
         <v>0</v>
@@ -2823,10 +2823,10 @@
         <v>0</v>
       </c>
       <c r="BV9" t="n">
-        <v>79.175</v>
+        <v>7.425</v>
       </c>
       <c r="BW9" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="BX9" t="n">
         <v>0</v>
@@ -2835,7 +2835,7 @@
         <v>0</v>
       </c>
       <c r="BZ9" t="n">
-        <v>76.425</v>
+        <v>0.025</v>
       </c>
       <c r="CA9" t="n">
         <v>0</v>
@@ -2847,10 +2847,10 @@
         <v>0</v>
       </c>
       <c r="CD9" t="n">
-        <v>2.75</v>
+        <v>7.4</v>
       </c>
       <c r="CE9" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>